<commit_message>
COST DRIVETRAIN : A0900 fini (33%)
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
+++ b/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Documents\ECL\EPSA\Github\EN - Engine &amp; Powertrain\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC37771-FD9B-45AD-8044-0563E20D0700}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EFA2BF-0518-4F50-88C9-A1F8D957BBF4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -25,13 +25,18 @@
     <sheet name="EN_0900_004" sheetId="14" r:id="rId9"/>
     <sheet name="EN_0900_004 Drawing" sheetId="23" r:id="rId10"/>
     <sheet name="EN_0900_005" sheetId="15" r:id="rId11"/>
-    <sheet name="EN_0900_006" sheetId="16" r:id="rId12"/>
-    <sheet name="EN_0900_007" sheetId="17" r:id="rId13"/>
-    <sheet name="EN_0900_008" sheetId="19" r:id="rId14"/>
-    <sheet name="EN_0900_009" sheetId="20" r:id="rId15"/>
+    <sheet name="EN_0900_005 Drawing" sheetId="24" r:id="rId12"/>
+    <sheet name="EN_0900_006" sheetId="16" r:id="rId13"/>
+    <sheet name="EN_0900_006 Drawing" sheetId="25" r:id="rId14"/>
+    <sheet name="EN_0900_007" sheetId="17" r:id="rId15"/>
+    <sheet name="EN_0900_007 Drawing" sheetId="26" r:id="rId16"/>
+    <sheet name="EN_0900_008" sheetId="19" r:id="rId17"/>
+    <sheet name="EN_0900_008 Drawing" sheetId="27" r:id="rId18"/>
+    <sheet name="EN_0900_009" sheetId="20" r:id="rId19"/>
+    <sheet name="EN_0900_009 Drawing" sheetId="28" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="_____________uni2">#REF!</definedName>
@@ -174,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="249">
   <si>
     <t>University</t>
   </si>
@@ -2374,6 +2379,202 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
+      <xdr:colOff>393872</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>170517</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91B9F1C7-A378-4716-9DDB-4B0B4ADA351C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12804947" y="2867024"/>
+          <a:ext cx="2824645" cy="2266201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>150886</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>27503</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{966836FC-CD9E-43CA-B2B8-F93372437CF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="600075"/>
+          <a:ext cx="12114286" cy="8571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>75451</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>94542</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DDF04F-B410-4463-A054-47A66011C9A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12973050" y="2733675"/>
+          <a:ext cx="2351926" cy="1932867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>293762</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>141803</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2C38CA7-6D69-4ACC-A010-D018B9429449}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="333375"/>
+          <a:ext cx="12104762" cy="8571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>419922</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
@@ -2418,7 +2619,56 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>693809</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>189428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5B1FB30-FAA5-46FF-BEC4-59C9430E8EA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="381000"/>
+          <a:ext cx="12123809" cy="8571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2456,6 +2706,55 @@
         <a:xfrm>
           <a:off x="12088123" y="2609849"/>
           <a:ext cx="1637401" cy="2145775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>693809</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>94178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F007648-4F4A-469B-ACDB-5EC10AB6469B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="476250"/>
+          <a:ext cx="12123809" cy="8571428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2716,6 +3015,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>65159</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>37028</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68A16B71-D05A-4ABF-BE69-811FA24349E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="228600"/>
+          <a:ext cx="12123809" cy="8571428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -2761,27 +3109,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>393872</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>170517</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>180225</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>131837</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>94178</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
+        <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91B9F1C7-A378-4716-9DDB-4B0B4ADA351C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90785991-D816-4A13-9208-5E67E33A948B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2797,57 +3145,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12804947" y="2867024"/>
-          <a:ext cx="2824645" cy="2266201"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>75451</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>94542</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03DDF04F-B410-4463-A054-47A66011C9A0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12973050" y="2733675"/>
-          <a:ext cx="2351926" cy="1932867"/>
+          <a:off x="219075" y="285750"/>
+          <a:ext cx="12104762" cy="8571428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3570,8 +3869,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,6 +3885,7 @@
     <hyperlink ref="A1" location="EN_0900_004" display="EN_0900_004" xr:uid="{2E4E2DB0-CD4F-4100-BC62-30408841A317}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3597,7 +3897,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,7 +3964,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="46"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="223" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -4262,20 +4562,50 @@
       <c r="O28" s="175"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" location="'EN_0900_005 Drawing'!A1" display="FileLink1" xr:uid="{61892D57-9684-4295-9529-3CA5DC00953C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD12B02-713E-4B1A-90B4-9B3E5C72B5DC}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_0900_005" display="EN_0900_005" xr:uid="{C4345D02-149F-4EAA-AEE8-2D8364388E73}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE1F031-A6B2-4C3F-B011-3A3FB7B7A2BE}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4343,7 +4673,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="46"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="223" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -4929,20 +5259,48 @@
       <c r="O27" s="175"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" location="'EN_0900_006 Drawing'!A1" display="FileLink1" xr:uid="{731B3E14-BD29-4A7B-8AEC-C7E1C65CD6EF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1C2C23-2CF0-4D1F-B54A-55E717260FC6}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_0900_006" display="EN_0900_006" xr:uid="{459E7C1C-6BD1-47EF-AA5D-C8488BE4679A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA90DC19-37A4-4EEE-84E9-C63D226B8D65}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5010,7 +5368,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="46"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="223" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -5579,12 +5937,40 @@
       <c r="O26" s="175"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" location="'EN_0900_007 Drawing'!A1" display="FileLink1" xr:uid="{456BD7D5-0F5C-4D47-BE9E-315D5EC71C92}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FCC624-E26D-4C77-98B2-9FCF568FF717}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_0900_007" display="EN_0900_007" xr:uid="{3D2D908B-3D39-40F3-A8B1-E3AA97A249D9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54503668-160D-42F8-9C78-2918A90FDF49}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -5592,7 +5978,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5660,7 +6046,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="46"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="223" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -6212,12 +6598,40 @@
       <c r="O25" s="175"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" location="'EN_0900_008 Drawing'!A1" display="FileLink1" xr:uid="{CF540C9A-7D70-4139-B381-37726EB07E31}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F4C775-5DF4-43D4-A248-EF81D0028773}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_0900_008" display="EN_0900_008" xr:uid="{5451F878-B3C6-4CD7-9CFD-DA94F1169DC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239B2C40-352C-4863-A7D8-A4EE5DA4B3A3}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -6225,7 +6639,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6293,7 +6707,7 @@
         <v>135</v>
       </c>
       <c r="C3" s="46"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="223" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="46" t="s">
@@ -6845,6 +7259,9 @@
       <c r="O25" s="175"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" location="'EN_0900_009 Drawing'!A1" display="FileLink1" xr:uid="{C0B6B514-8E88-4C67-A76D-070A1E227D85}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -9608,6 +10025,33 @@
   <ignoredErrors>
     <ignoredError sqref="H8:M8 H9:H17 C7:C8 I7:M7" unlockedFormula="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720CD844-52BF-4DAC-8E45-9D6F7FAE85A7}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_0900_009" display="EN_0900_009" xr:uid="{35F4E745-4FD9-40E4-8E32-5B4E844C3F5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14211,7 +14655,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -14239,7 +14683,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
COST DRIVETRAIN : 60% (revoir axles) + reste Chain set
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
+++ b/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Documents\ECL\EPSA\Github\EN - Engine &amp; Powertrain\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3488F85C-76F5-4F54-8B5B-CDFC572F01C8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8E82EF-3999-49B6-9B28-6D7366D5D7C7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="16" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="21" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -36,12 +36,16 @@
     <sheet name="EN_0900_009 Drawing" sheetId="28" r:id="rId20"/>
     <sheet name="EN_A1000" sheetId="29" r:id="rId21"/>
     <sheet name="EN_1000_001" sheetId="30" r:id="rId22"/>
+    <sheet name="EN_1000_002" sheetId="32" r:id="rId23"/>
+    <sheet name="EN_1000_003" sheetId="34" r:id="rId24"/>
+    <sheet name="EN_1000_003 Drawing" sheetId="37" r:id="rId25"/>
+    <sheet name="EN_1000_004" sheetId="33" r:id="rId26"/>
+    <sheet name="EN_1000_004 Drawing" sheetId="38" r:id="rId27"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId23"/>
-    <externalReference r:id="rId24"/>
-    <externalReference r:id="rId25"/>
-    <externalReference r:id="rId26"/>
+    <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
   </externalReferences>
   <definedNames>
     <definedName name="_____________uni2">#REF!</definedName>
@@ -122,8 +126,20 @@
     <definedName name="EN_0900_009_q">EN_0900_009!$N$3</definedName>
     <definedName name="EN_1000_001">EN_1000_001!$B$6</definedName>
     <definedName name="EN_1000_001_m">EN_1000_001!$N$13</definedName>
-    <definedName name="EN_1000_001_p">EN_1000_001!$I$20</definedName>
+    <definedName name="EN_1000_001_p">EN_1000_001!$I$22</definedName>
     <definedName name="EN_1000_001_q">EN_1000_001!$N$3</definedName>
+    <definedName name="EN_1000_002">EN_1000_002!$B$6</definedName>
+    <definedName name="EN_1000_002_m">EN_1000_002!$N$12</definedName>
+    <definedName name="EN_1000_002_p">EN_1000_002!$I$23</definedName>
+    <definedName name="EN_1000_002_q">EN_1000_002!$N$3</definedName>
+    <definedName name="EN_1000_003">EN_1000_003!$B$6</definedName>
+    <definedName name="EN_1000_003_m">EN_1000_003!$N$12</definedName>
+    <definedName name="EN_1000_003_p">EN_1000_003!$I$21</definedName>
+    <definedName name="EN_1000_003_q">EN_1000_003!$N$3</definedName>
+    <definedName name="EN_1000_004">EN_1000_004!$B$6</definedName>
+    <definedName name="EN_1000_004_m">EN_1000_004!$N$13</definedName>
+    <definedName name="EN_1000_004_p">EN_1000_004!$I$21</definedName>
+    <definedName name="EN_1000_004_q">EN_1000_004!$N$3</definedName>
     <definedName name="EN_A0900">EN_A0900!$B$5</definedName>
     <definedName name="EN_A0900_f">EN_A0900!$J$56</definedName>
     <definedName name="EN_A0900_m">EN_A0900!$N$27</definedName>
@@ -188,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="308">
   <si>
     <t>University</t>
   </si>
@@ -1086,26 +1102,83 @@
     <t>Setup and removal of the machining of the tripod housing</t>
   </si>
   <si>
-    <t>Shaping of the tripod housing</t>
-  </si>
-  <si>
     <t>Material-Steel</t>
   </si>
   <si>
     <t>Machining Setup, Change</t>
   </si>
   <si>
-    <t>Setup and removal of the broach of the tripod housing</t>
-  </si>
-  <si>
     <t>Broach of the tripod housing</t>
+  </si>
+  <si>
+    <t>Machining the ext shape of the tripod housing (turning)</t>
+  </si>
+  <si>
+    <t>Material - Steel</t>
+  </si>
+  <si>
+    <t>Machining the int shape of the tripod housing (milling)</t>
+  </si>
+  <si>
+    <t>Changing of the machining of the tripod housing</t>
+  </si>
+  <si>
+    <t>Changing of the broach of the tripod housing</t>
+  </si>
+  <si>
+    <t>EN_1000_002</t>
+  </si>
+  <si>
+    <t>EN_1000_003</t>
+  </si>
+  <si>
+    <t>Left Axle</t>
+  </si>
+  <si>
+    <t>Right Axle</t>
+  </si>
+  <si>
+    <t>EN_1000_004</t>
+  </si>
+  <si>
+    <t>Setup and removal of the threading of the tripod housing</t>
+  </si>
+  <si>
+    <t>Threading, External (machining)</t>
+  </si>
+  <si>
+    <t>Threading of the tripod housing</t>
+  </si>
+  <si>
+    <t>Round 22,1 mm diam.</t>
+  </si>
+  <si>
+    <t>Material for driveshaft</t>
+  </si>
+  <si>
+    <t>Setup and removal of the machining of the axle</t>
+  </si>
+  <si>
+    <t>Setup and removal of the broach of the axle</t>
+  </si>
+  <si>
+    <t>Broach of the axle</t>
+  </si>
+  <si>
+    <t>Cut of the edge of the axle</t>
+  </si>
+  <si>
+    <t>Shaping of the int of the axle</t>
+  </si>
+  <si>
+    <t>Drawing of the cut</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="15">
+  <numFmts count="17">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
@@ -1121,6 +1194,8 @@
     <numFmt numFmtId="174" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
     <numFmt numFmtId="175" formatCode="0.0000E+00"/>
     <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="180" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -1365,7 +1440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -2028,6 +2103,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2053,7 +2197,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -2424,7 +2568,6 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="24" fillId="0" borderId="50" xfId="12" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="24" fillId="0" borderId="52" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2435,7 +2578,6 @@
     <xf numFmtId="172" fontId="24" fillId="0" borderId="52" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="24" fillId="0" borderId="52" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="24" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="52" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="39" fontId="24" fillId="0" borderId="52" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="24" fillId="0" borderId="52" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2458,12 +2600,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="24" fillId="0" borderId="52" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="24" fillId="0" borderId="52" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="11" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="52" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2478,6 +2614,74 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="53" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="55" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="57" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="54" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="57" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="10" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="24" fillId="0" borderId="54" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="58" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3042,6 +3246,104 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>458372</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>131763</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>55790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80E1E7AE-3F3C-465D-BFDA-0E7C034EE704}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14342460" y="2667000"/>
+          <a:ext cx="3483391" cy="2722790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>591792</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>589559</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>46821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB0DB1D4-A93F-47DC-B712-02714B82B549}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12498042" y="2657475"/>
+          <a:ext cx="3121967" cy="2532846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3080,6 +3382,104 @@
         <a:xfrm>
           <a:off x="9929842" y="2771775"/>
           <a:ext cx="2518187" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584864</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>579917</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>18332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E7E2411-C110-464B-8EC9-80A06A754A05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11805314" y="2428875"/>
+          <a:ext cx="3043053" cy="1970957"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>18476</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>46926</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17B2ADF5-BFF8-4D8A-9C36-723CED200E25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11706225" y="2628900"/>
+          <a:ext cx="3342701" cy="1990026"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3472,7 +3872,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="EN_1000_002"/>
+      <sheetName val="EN_1000_003"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -3482,19 +3882,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="EN_1000_003"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6957,8 +7344,8 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:O25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10380,8 +10767,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10580,7 +10967,7 @@
       <c r="A9" s="227" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="247" t="s">
+      <c r="B9" s="245" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="228" t="s">
@@ -10607,20 +10994,20 @@
       <c r="A10" s="230">
         <v>10</v>
       </c>
-      <c r="B10" s="266" t="s">
+      <c r="B10" s="260" t="s">
         <v>250</v>
       </c>
       <c r="C10" s="229">
         <f>EN_1000_001!N$2</f>
-        <v>67.057360933677941</v>
-      </c>
-      <c r="D10" s="232">
+        <v>66.549787154500507</v>
+      </c>
+      <c r="D10" s="231">
         <f>EN_1000_001_q</f>
         <v>2</v>
       </c>
-      <c r="E10" s="233">
+      <c r="E10" s="232">
         <f>C10*D10</f>
-        <v>134.11472186735588</v>
+        <v>133.09957430900101</v>
       </c>
       <c r="F10" s="111"/>
       <c r="G10" s="111"/>
@@ -10637,18 +11024,18 @@
       <c r="A11" s="230">
         <v>20</v>
       </c>
-      <c r="B11" s="231" t="s">
+      <c r="B11" s="260" t="s">
         <v>251</v>
       </c>
       <c r="C11" s="229" t="e">
-        <f>[2]EN_1000_002!N$2</f>
+        <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="232" t="e">
-        <f>EN_1000_002_m</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E11" s="233" t="e">
+      <c r="D11" s="231">
+        <f>EN_1000_002_q</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="232" t="e">
         <f>C11*D11</f>
         <v>#REF!</v>
       </c>
@@ -10667,18 +11054,18 @@
       <c r="A12" s="230">
         <v>30</v>
       </c>
-      <c r="B12" s="231" t="s">
+      <c r="B12" s="286" t="s">
         <v>253</v>
       </c>
       <c r="C12" s="229" t="e">
-        <f>[3]EN_1000_003!N$2</f>
+        <f>[2]EN_1000_003!N$2</f>
         <v>#REF!</v>
       </c>
-      <c r="D12" s="232" t="e">
-        <f>EN_1000_003_m</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E12" s="233" t="e">
+      <c r="D12" s="231">
+        <f>EN_1000_003_q</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="232" t="e">
         <f>C12*D12</f>
         <v>#REF!</v>
       </c>
@@ -10697,18 +11084,18 @@
       <c r="A13" s="230">
         <v>40</v>
       </c>
-      <c r="B13" s="231" t="s">
+      <c r="B13" s="260" t="s">
         <v>252</v>
       </c>
       <c r="C13" s="229" t="e">
-        <f>[4]EN_1000_004!N$2</f>
+        <f>[3]EN_1000_004!N$2</f>
         <v>#REF!</v>
       </c>
-      <c r="D13" s="232" t="e">
+      <c r="D13" s="231">
         <f>EN_1000_004_q</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E13" s="233" t="e">
+        <v>2</v>
+      </c>
+      <c r="E13" s="232" t="e">
         <f>C13*D13</f>
         <v>#REF!</v>
       </c>
@@ -10808,64 +11195,64 @@
       <c r="O16" s="167"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="234">
+      <c r="A17" s="233">
         <v>10</v>
       </c>
-      <c r="B17" s="235" t="s">
+      <c r="B17" s="234" t="s">
         <v>254</v>
       </c>
-      <c r="C17" s="235" t="s">
+      <c r="C17" s="234" t="s">
         <v>255</v>
       </c>
-      <c r="D17" s="236">
+      <c r="D17" s="235">
         <v>45</v>
       </c>
-      <c r="E17" s="235"/>
-      <c r="F17" s="235" t="s">
+      <c r="E17" s="234"/>
+      <c r="F17" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="235"/>
-      <c r="H17" s="237"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="239"/>
-      <c r="K17" s="237"/>
-      <c r="L17" s="237"/>
-      <c r="M17" s="239">
+      <c r="G17" s="234"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="237"/>
+      <c r="J17" s="238"/>
+      <c r="K17" s="236"/>
+      <c r="L17" s="236"/>
+      <c r="M17" s="238">
         <v>4</v>
       </c>
-      <c r="N17" s="240">
+      <c r="N17" s="239">
         <f>IF(J17="",D17*M17,D17*J17*K17*L17*M17)</f>
         <v>180</v>
       </c>
       <c r="O17" s="170"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="234">
+      <c r="A18" s="233">
         <v>20</v>
       </c>
-      <c r="B18" s="235" t="s">
+      <c r="B18" s="234" t="s">
         <v>256</v>
       </c>
-      <c r="C18" s="235" t="s">
+      <c r="C18" s="234" t="s">
         <v>257</v>
       </c>
-      <c r="D18" s="236">
+      <c r="D18" s="235">
         <v>5</v>
       </c>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235" t="s">
+      <c r="E18" s="234"/>
+      <c r="F18" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="235"/>
-      <c r="H18" s="237"/>
-      <c r="I18" s="238"/>
-      <c r="J18" s="239"/>
-      <c r="K18" s="237"/>
-      <c r="L18" s="237"/>
-      <c r="M18" s="239">
+      <c r="G18" s="234"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="237"/>
+      <c r="J18" s="238"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="236"/>
+      <c r="M18" s="238">
         <v>4</v>
       </c>
-      <c r="N18" s="240">
+      <c r="N18" s="239">
         <f>IF(J18="",D18*M18,D18*J18*K18*L18*M18)</f>
         <v>20</v>
       </c>
@@ -10946,29 +11333,29 @@
       <c r="O21" s="163"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="234">
+      <c r="A22" s="233">
         <v>10</v>
       </c>
-      <c r="B22" s="232" t="s">
+      <c r="B22" s="231" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="232" t="s">
+      <c r="C22" s="231" t="s">
         <v>258</v>
       </c>
-      <c r="D22" s="236">
+      <c r="D22" s="235">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E22" s="235" t="s">
+      <c r="E22" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="235">
+      <c r="F22" s="234">
         <v>2</v>
       </c>
-      <c r="G22" s="235"/>
-      <c r="H22" s="235">
+      <c r="G22" s="234"/>
+      <c r="H22" s="234">
         <v>1</v>
       </c>
-      <c r="I22" s="236">
+      <c r="I22" s="235">
         <f t="shared" ref="I22:I33" si="0">D22*F22*H22</f>
         <v>1.1200000000000001</v>
       </c>
@@ -10980,29 +11367,29 @@
       <c r="O22" s="163"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="234">
+      <c r="A23" s="233">
         <v>20</v>
       </c>
-      <c r="B23" s="232" t="s">
+      <c r="B23" s="231" t="s">
         <v>259</v>
       </c>
-      <c r="C23" s="232" t="s">
+      <c r="C23" s="231" t="s">
         <v>260</v>
       </c>
-      <c r="D23" s="236">
+      <c r="D23" s="235">
         <v>1.5</v>
       </c>
-      <c r="E23" s="235" t="s">
+      <c r="E23" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="235">
+      <c r="F23" s="234">
         <v>2</v>
       </c>
-      <c r="G23" s="235"/>
-      <c r="H23" s="235">
+      <c r="G23" s="234"/>
+      <c r="H23" s="234">
         <v>1</v>
       </c>
-      <c r="I23" s="236">
+      <c r="I23" s="235">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -11014,29 +11401,29 @@
       <c r="O23" s="163"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="234">
+      <c r="A24" s="233">
         <v>30</v>
       </c>
-      <c r="B24" s="232" t="s">
+      <c r="B24" s="231" t="s">
         <v>188</v>
       </c>
-      <c r="C24" s="232" t="s">
+      <c r="C24" s="231" t="s">
         <v>261</v>
       </c>
-      <c r="D24" s="236">
+      <c r="D24" s="235">
         <v>0.19</v>
       </c>
-      <c r="E24" s="235" t="s">
+      <c r="E24" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="235">
+      <c r="F24" s="234">
         <v>4</v>
       </c>
-      <c r="G24" s="235"/>
-      <c r="H24" s="235">
+      <c r="G24" s="234"/>
+      <c r="H24" s="234">
         <v>1</v>
       </c>
-      <c r="I24" s="236">
+      <c r="I24" s="235">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -11048,29 +11435,29 @@
       <c r="O24" s="163"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="234">
+      <c r="A25" s="233">
         <v>40</v>
       </c>
-      <c r="B25" s="232" t="s">
+      <c r="B25" s="231" t="s">
         <v>188</v>
       </c>
-      <c r="C25" s="232" t="s">
+      <c r="C25" s="231" t="s">
         <v>262</v>
       </c>
-      <c r="D25" s="236">
+      <c r="D25" s="235">
         <v>0.19</v>
       </c>
-      <c r="E25" s="235" t="s">
+      <c r="E25" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="235">
+      <c r="F25" s="234">
         <v>4</v>
       </c>
-      <c r="G25" s="235"/>
-      <c r="H25" s="235">
+      <c r="G25" s="234"/>
+      <c r="H25" s="234">
         <v>1</v>
       </c>
-      <c r="I25" s="236">
+      <c r="I25" s="235">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -11082,29 +11469,29 @@
       <c r="O25" s="163"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="234">
+      <c r="A26" s="233">
         <v>50</v>
       </c>
-      <c r="B26" s="232" t="s">
+      <c r="B26" s="231" t="s">
         <v>173</v>
       </c>
-      <c r="C26" s="232" t="s">
+      <c r="C26" s="231" t="s">
         <v>263</v>
       </c>
-      <c r="D26" s="236">
+      <c r="D26" s="235">
         <v>0.13</v>
       </c>
-      <c r="E26" s="235" t="s">
+      <c r="E26" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="235">
+      <c r="F26" s="234">
         <v>4</v>
       </c>
-      <c r="G26" s="235"/>
-      <c r="H26" s="235">
+      <c r="G26" s="234"/>
+      <c r="H26" s="234">
         <v>1</v>
       </c>
-      <c r="I26" s="236">
+      <c r="I26" s="235">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
@@ -11116,29 +11503,29 @@
       <c r="O26" s="170"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="234">
+      <c r="A27" s="233">
         <v>60</v>
       </c>
-      <c r="B27" s="232" t="s">
+      <c r="B27" s="231" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="232" t="s">
+      <c r="C27" s="231" t="s">
         <v>262</v>
       </c>
-      <c r="D27" s="236">
+      <c r="D27" s="235">
         <v>0.19</v>
       </c>
-      <c r="E27" s="235" t="s">
+      <c r="E27" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="235">
+      <c r="F27" s="234">
         <v>4</v>
       </c>
-      <c r="G27" s="235"/>
-      <c r="H27" s="235">
+      <c r="G27" s="234"/>
+      <c r="H27" s="234">
         <v>1</v>
       </c>
-      <c r="I27" s="236">
+      <c r="I27" s="235">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -11150,29 +11537,29 @@
       <c r="O27" s="163"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="234">
+      <c r="A28" s="233">
         <v>70</v>
       </c>
-      <c r="B28" s="232" t="s">
+      <c r="B28" s="231" t="s">
         <v>264</v>
       </c>
-      <c r="C28" s="232" t="s">
+      <c r="C28" s="231" t="s">
         <v>265</v>
       </c>
-      <c r="D28" s="236">
+      <c r="D28" s="235">
         <v>0.19</v>
       </c>
-      <c r="E28" s="235" t="s">
+      <c r="E28" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="235">
+      <c r="F28" s="234">
         <v>4</v>
       </c>
-      <c r="G28" s="235"/>
-      <c r="H28" s="235">
+      <c r="G28" s="234"/>
+      <c r="H28" s="234">
         <v>1</v>
       </c>
-      <c r="I28" s="236">
+      <c r="I28" s="235">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -11184,29 +11571,29 @@
       <c r="O28" s="163"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="234">
+      <c r="A29" s="233">
         <v>80</v>
       </c>
-      <c r="B29" s="232" t="s">
+      <c r="B29" s="231" t="s">
         <v>188</v>
       </c>
-      <c r="C29" s="232" t="s">
+      <c r="C29" s="231" t="s">
         <v>266</v>
       </c>
-      <c r="D29" s="236">
+      <c r="D29" s="235">
         <v>0.19</v>
       </c>
-      <c r="E29" s="235" t="s">
+      <c r="E29" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="235">
+      <c r="F29" s="234">
         <v>4</v>
       </c>
-      <c r="G29" s="235"/>
-      <c r="H29" s="235">
+      <c r="G29" s="234"/>
+      <c r="H29" s="234">
         <v>1</v>
       </c>
-      <c r="I29" s="236">
+      <c r="I29" s="235">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -11218,29 +11605,29 @@
       <c r="O29" s="163"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="234">
+      <c r="A30" s="233">
         <v>90</v>
       </c>
-      <c r="B30" s="232" t="s">
+      <c r="B30" s="231" t="s">
         <v>186</v>
       </c>
-      <c r="C30" s="232" t="s">
+      <c r="C30" s="231" t="s">
         <v>267</v>
       </c>
-      <c r="D30" s="236">
+      <c r="D30" s="235">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E30" s="235" t="s">
+      <c r="E30" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="235">
+      <c r="F30" s="234">
         <v>2</v>
       </c>
-      <c r="G30" s="235"/>
-      <c r="H30" s="235">
+      <c r="G30" s="234"/>
+      <c r="H30" s="234">
         <v>1</v>
       </c>
-      <c r="I30" s="236">
+      <c r="I30" s="235">
         <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
@@ -11252,29 +11639,29 @@
       <c r="O30" s="163"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="234">
+      <c r="A31" s="233">
         <v>100</v>
       </c>
-      <c r="B31" s="232" t="s">
+      <c r="B31" s="231" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="232" t="s">
+      <c r="C31" s="231" t="s">
         <v>271</v>
       </c>
-      <c r="D31" s="236">
+      <c r="D31" s="235">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E31" s="235" t="s">
+      <c r="E31" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="235">
+      <c r="F31" s="234">
         <v>4</v>
       </c>
-      <c r="G31" s="235"/>
-      <c r="H31" s="235">
+      <c r="G31" s="234"/>
+      <c r="H31" s="234">
         <v>1</v>
       </c>
-      <c r="I31" s="236">
+      <c r="I31" s="235">
         <f t="shared" si="0"/>
         <v>2.2400000000000002</v>
       </c>
@@ -11286,29 +11673,29 @@
       <c r="O31" s="163"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="234">
+      <c r="A32" s="233">
         <v>110</v>
       </c>
-      <c r="B32" s="232" t="s">
+      <c r="B32" s="231" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="232" t="s">
+      <c r="C32" s="231" t="s">
         <v>270</v>
       </c>
-      <c r="D32" s="236">
+      <c r="D32" s="235">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E32" s="235" t="s">
+      <c r="E32" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="235">
+      <c r="F32" s="234">
         <v>4</v>
       </c>
-      <c r="G32" s="235"/>
-      <c r="H32" s="235">
+      <c r="G32" s="234"/>
+      <c r="H32" s="234">
         <v>1</v>
       </c>
-      <c r="I32" s="236">
+      <c r="I32" s="235">
         <f t="shared" si="0"/>
         <v>2.2400000000000002</v>
       </c>
@@ -11320,29 +11707,29 @@
       <c r="O32" s="163"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="234">
+      <c r="A33" s="233">
         <v>120</v>
       </c>
-      <c r="B33" s="232" t="s">
+      <c r="B33" s="231" t="s">
         <v>268</v>
       </c>
-      <c r="C33" s="232" t="s">
+      <c r="C33" s="231" t="s">
         <v>269</v>
       </c>
-      <c r="D33" s="236">
+      <c r="D33" s="235">
         <v>0.75</v>
       </c>
-      <c r="E33" s="235" t="s">
+      <c r="E33" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="235">
+      <c r="F33" s="234">
         <v>2</v>
       </c>
-      <c r="G33" s="235"/>
-      <c r="H33" s="235">
+      <c r="G33" s="234"/>
+      <c r="H33" s="234">
         <v>1</v>
       </c>
-      <c r="I33" s="236">
+      <c r="I33" s="235">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
@@ -11430,31 +11817,31 @@
       <c r="O36" s="163"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="234">
+      <c r="A37" s="233">
         <v>10</v>
       </c>
-      <c r="B37" s="235" t="s">
+      <c r="B37" s="234" t="s">
         <v>272</v>
       </c>
-      <c r="C37" s="235" t="s">
+      <c r="C37" s="234" t="s">
         <v>273</v>
       </c>
-      <c r="D37" s="241">
+      <c r="D37" s="240">
         <f>0.0002*E37*E37+0.013</f>
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E37" s="235">
+      <c r="E37" s="234">
         <v>20</v>
       </c>
-      <c r="F37" s="243" t="s">
+      <c r="F37" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="235"/>
-      <c r="H37" s="232"/>
-      <c r="I37" s="244">
+      <c r="G37" s="234"/>
+      <c r="H37" s="231"/>
+      <c r="I37" s="242">
         <v>8</v>
       </c>
-      <c r="J37" s="236">
+      <c r="J37" s="235">
         <f>D37*I37</f>
         <v>0.74399999999999999</v>
       </c>
@@ -11465,32 +11852,32 @@
       <c r="O37" s="163"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="234">
+      <c r="A38" s="233">
         <v>20</v>
       </c>
-      <c r="B38" s="245" t="s">
+      <c r="B38" s="243" t="s">
         <v>274</v>
       </c>
-      <c r="C38" s="235" t="s">
+      <c r="C38" s="234" t="s">
         <v>275</v>
       </c>
-      <c r="D38" s="241">
+      <c r="D38" s="240">
         <f>0.004*E38+0.5</f>
         <v>0.7898639999999999</v>
       </c>
-      <c r="E38" s="235">
+      <c r="E38" s="234">
         <f>36.233*2</f>
         <v>72.465999999999994</v>
       </c>
-      <c r="F38" s="243" t="s">
+      <c r="F38" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="235"/>
-      <c r="H38" s="232"/>
-      <c r="I38" s="244">
+      <c r="G38" s="234"/>
+      <c r="H38" s="231"/>
+      <c r="I38" s="242">
         <v>4</v>
       </c>
-      <c r="J38" s="236">
+      <c r="J38" s="235">
         <f>D38*I38</f>
         <v>3.1594559999999996</v>
       </c>
@@ -11501,32 +11888,32 @@
       <c r="O38" s="163"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="234">
+      <c r="A39" s="233">
         <v>30</v>
       </c>
-      <c r="B39" s="245" t="s">
+      <c r="B39" s="243" t="s">
         <v>274</v>
       </c>
-      <c r="C39" s="235" t="s">
+      <c r="C39" s="234" t="s">
         <v>275</v>
       </c>
-      <c r="D39" s="241">
+      <c r="D39" s="240">
         <f>0.004*E39+0.5</f>
         <v>0.61115200000000003</v>
       </c>
-      <c r="E39" s="235">
+      <c r="E39" s="234">
         <f>13.894*2</f>
         <v>27.788</v>
       </c>
-      <c r="F39" s="243" t="s">
+      <c r="F39" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="235"/>
-      <c r="H39" s="232"/>
-      <c r="I39" s="244">
+      <c r="G39" s="234"/>
+      <c r="H39" s="231"/>
+      <c r="I39" s="242">
         <v>4</v>
       </c>
-      <c r="J39" s="236">
+      <c r="J39" s="235">
         <f>D39*I39</f>
         <v>2.4446080000000001</v>
       </c>
@@ -11537,35 +11924,35 @@
       <c r="O39" s="163"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="234">
+      <c r="A40" s="233">
         <v>40</v>
       </c>
-      <c r="B40" s="235" t="s">
+      <c r="B40" s="234" t="s">
         <v>203</v>
       </c>
-      <c r="C40" s="235" t="s">
+      <c r="C40" s="234" t="s">
         <v>276</v>
       </c>
-      <c r="D40" s="241">
+      <c r="D40" s="240">
         <f>0.8/105154*E40*E40*G40*SQRT(G40)+(0.003*EXP(0.319*E40))</f>
         <v>8.2048330888522564E-2</v>
       </c>
-      <c r="E40" s="235">
+      <c r="E40" s="234">
         <v>8</v>
       </c>
-      <c r="F40" s="243" t="s">
+      <c r="F40" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="235">
+      <c r="G40" s="234">
         <v>20</v>
       </c>
-      <c r="H40" s="232" t="s">
+      <c r="H40" s="231" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="244">
+      <c r="I40" s="242">
         <v>2</v>
       </c>
-      <c r="J40" s="236">
+      <c r="J40" s="235">
         <f>D40*I40</f>
         <v>0.16409666177704513</v>
       </c>
@@ -11576,30 +11963,30 @@
       <c r="O40" s="163"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="234">
+      <c r="A41" s="233">
         <v>50</v>
       </c>
-      <c r="B41" s="246" t="s">
+      <c r="B41" s="244" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="235" t="s">
+      <c r="C41" s="234" t="s">
         <v>278</v>
       </c>
-      <c r="D41" s="241">
+      <c r="D41" s="240">
         <v>0.49</v>
       </c>
-      <c r="E41" s="235">
+      <c r="E41" s="234">
         <v>20</v>
       </c>
-      <c r="F41" s="243" t="s">
+      <c r="F41" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="235"/>
-      <c r="H41" s="232"/>
-      <c r="I41" s="244">
+      <c r="G41" s="234"/>
+      <c r="H41" s="231"/>
+      <c r="I41" s="242">
         <v>2</v>
       </c>
-      <c r="J41" s="236">
+      <c r="J41" s="235">
         <f>D41*I41</f>
         <v>0.98</v>
       </c>
@@ -11668,6 +12055,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" location="EN_1000_001!A1" display="Inboard tripod housing" xr:uid="{A72A27D6-2A20-4300-924D-C758BA327F7E}"/>
+    <hyperlink ref="B11" location="EN_1000_002!A1" display="Outboard tripod housing" xr:uid="{F3F51DEF-8CFB-40F9-85B6-42EB9AFF8C62}"/>
+    <hyperlink ref="B13" location="EN_1000_004!A1" display="Right axle" xr:uid="{F9A1E856-B4CC-4119-A1D5-7D5CC7E17549}"/>
+    <hyperlink ref="B12" location="EN_1000_003!A1" display="Left axle" xr:uid="{B3F2C828-FBF9-4C6B-8B62-07309ADDA238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11678,17 +12068,19 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11737,7 +12129,7 @@
       </c>
       <c r="N2" s="61">
         <f>EN_1000_001_m+EN_1000_001_p</f>
-        <v>67.057360933677941</v>
+        <v>66.549787154500507</v>
       </c>
       <c r="O2" s="163"/>
     </row>
@@ -11749,7 +12141,7 @@
         <v>134</v>
       </c>
       <c r="C3" s="45"/>
-      <c r="D3" s="258" t="s">
+      <c r="D3" s="252" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="45" t="s">
@@ -11771,10 +12163,10 @@
       <c r="O3" s="163"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="253" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="260" t="s">
+      <c r="B4" s="254" t="s">
         <v>249</v>
       </c>
       <c r="C4" s="45"/>
@@ -11796,7 +12188,7 @@
       <c r="O4" s="163"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="253" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="226" t="s">
@@ -11821,12 +12213,12 @@
       </c>
       <c r="N5" s="61">
         <f>N3*N2</f>
-        <v>134.11472186735588</v>
+        <v>133.09957430900101</v>
       </c>
       <c r="O5" s="163"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="259" t="s">
+      <c r="A6" s="253" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="175" t="s">
@@ -11921,31 +12313,31 @@
       <c r="E10" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="261" t="s">
+      <c r="F10" s="255" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="261" t="s">
+      <c r="G10" s="255" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="261" t="s">
+      <c r="H10" s="255" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="261" t="s">
+      <c r="I10" s="255" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="261" t="s">
+      <c r="J10" s="255" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="261" t="s">
+      <c r="K10" s="255" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="261" t="s">
+      <c r="L10" s="255" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="261" t="s">
+      <c r="M10" s="255" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="261" t="s">
+      <c r="N10" s="255" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="163"/>
@@ -11954,7 +12346,7 @@
       <c r="A11" s="187">
         <v>10</v>
       </c>
-      <c r="B11" s="245" t="s">
+      <c r="B11" s="243" t="s">
         <v>280</v>
       </c>
       <c r="C11" s="139" t="s">
@@ -11965,7 +12357,7 @@
       </c>
       <c r="E11" s="141">
         <f>J11*K11*L11</f>
-        <v>4.2321604149679732</v>
+        <v>4.0999054020002239</v>
       </c>
       <c r="F11" s="139" t="s">
         <v>155</v>
@@ -11980,7 +12372,7 @@
         <v>3.3695544705159026E-3</v>
       </c>
       <c r="K11" s="144">
-        <v>0.16</v>
+        <v>0.155</v>
       </c>
       <c r="L11" s="145">
         <v>7850</v>
@@ -11990,7 +12382,7 @@
       </c>
       <c r="N11" s="140">
         <f>D11*J11*K11*L11*M11</f>
-        <v>9.5223609336779393</v>
+        <v>9.224787154500504</v>
       </c>
       <c r="O11" s="167"/>
     </row>
@@ -12007,7 +12399,7 @@
       <c r="J12" s="134"/>
       <c r="K12" s="135"/>
       <c r="L12" s="136"/>
-      <c r="M12" s="262"/>
+      <c r="M12" s="256"/>
       <c r="N12" s="137"/>
       <c r="O12" s="167"/>
     </row>
@@ -12024,12 +12416,12 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="257" t="s">
         <v>18</v>
       </c>
       <c r="N13" s="105">
         <f>SUM(N11:N11)</f>
-        <v>9.5223609336779393</v>
+        <v>9.224787154500504</v>
       </c>
       <c r="O13" s="163"/>
     </row>
@@ -12051,31 +12443,31 @@
       <c r="O14" s="163"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="259" t="s">
+      <c r="A15" s="253" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="261" t="s">
+      <c r="B15" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="261" t="s">
+      <c r="C15" s="255" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="261" t="s">
+      <c r="D15" s="255" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="261" t="s">
+      <c r="E15" s="255" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="261" t="s">
+      <c r="F15" s="255" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="261" t="s">
+      <c r="G15" s="255" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="261" t="s">
+      <c r="H15" s="255" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="261" t="s">
+      <c r="I15" s="255" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="19"/>
@@ -12085,28 +12477,28 @@
       <c r="N15" s="19"/>
       <c r="O15" s="163"/>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="264">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="258">
         <v>10</v>
       </c>
-      <c r="B16" s="249" t="s">
+      <c r="B16" s="247" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="250" t="s">
+      <c r="C16" s="248" t="s">
         <v>283</v>
       </c>
-      <c r="D16" s="251">
+      <c r="D16" s="249">
         <v>1.3</v>
       </c>
-      <c r="E16" s="249" t="s">
+      <c r="E16" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="248">
+      <c r="F16" s="246">
         <v>1</v>
       </c>
-      <c r="G16" s="248"/>
-      <c r="H16" s="248"/>
-      <c r="I16" s="252">
+      <c r="G16" s="246"/>
+      <c r="H16" s="246"/>
+      <c r="I16" s="250">
         <f>IF(H16="",D16*F16,D16*F16*H16)</f>
         <v>1.3</v>
       </c>
@@ -12118,33 +12510,33 @@
       <c r="O16" s="163"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="265">
+      <c r="A17" s="259">
         <v>20</v>
       </c>
-      <c r="B17" s="250" t="s">
+      <c r="B17" s="248" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="250" t="s">
-        <v>284</v>
-      </c>
-      <c r="D17" s="242">
+      <c r="C17" s="248" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" s="249">
         <v>0.04</v>
       </c>
-      <c r="E17" s="253" t="s">
+      <c r="E17" s="263" t="s">
         <v>162</v>
       </c>
-      <c r="F17" s="254">
-        <v>453</v>
-      </c>
-      <c r="G17" s="255" t="s">
-        <v>285</v>
-      </c>
-      <c r="H17" s="256">
+      <c r="F17" s="251">
+        <v>269.89999999999998</v>
+      </c>
+      <c r="G17" s="265" t="s">
+        <v>288</v>
+      </c>
+      <c r="H17" s="266">
         <v>3</v>
       </c>
-      <c r="I17" s="252">
-        <f>IF(H17="",D17*F17,D17*F17*H17)</f>
-        <v>54.36</v>
+      <c r="I17" s="250">
+        <f t="shared" ref="I17:I21" si="0">IF(H17="",D17*F17,D17*F17*H17)</f>
+        <v>32.387999999999998</v>
       </c>
       <c r="J17" s="45"/>
       <c r="K17" s="45"/>
@@ -12154,28 +12546,28 @@
       <c r="O17" s="163"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="264">
+      <c r="A18" s="258">
         <v>30</v>
       </c>
-      <c r="B18" s="250" t="s">
-        <v>286</v>
-      </c>
-      <c r="C18" s="250" t="s">
-        <v>287</v>
-      </c>
-      <c r="D18" s="242">
+      <c r="B18" s="247" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="248" t="s">
+        <v>290</v>
+      </c>
+      <c r="D18" s="249">
         <v>0.65</v>
       </c>
-      <c r="E18" s="249" t="s">
+      <c r="E18" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="256">
+      <c r="F18" s="246">
         <v>1</v>
       </c>
-      <c r="G18" s="256"/>
-      <c r="H18" s="256"/>
-      <c r="I18" s="252">
-        <f>IF(H18="",D18*F18,D18*F18*H18)</f>
+      <c r="G18" s="246"/>
+      <c r="H18" s="246"/>
+      <c r="I18" s="250">
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="J18" s="45"/>
@@ -12186,29 +12578,33 @@
       <c r="O18" s="163"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="265">
+      <c r="A19" s="268">
         <v>40</v>
       </c>
-      <c r="B19" s="250" t="s">
-        <v>170</v>
-      </c>
-      <c r="C19" s="250" t="s">
+      <c r="B19" s="269" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="269" t="s">
+        <v>289</v>
+      </c>
+      <c r="D19" s="249">
+        <v>0.04</v>
+      </c>
+      <c r="E19" s="270" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="278">
+        <v>175.85</v>
+      </c>
+      <c r="G19" s="265" t="s">
         <v>288</v>
       </c>
-      <c r="D19" s="242">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="253" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="257">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="G19" s="249"/>
-      <c r="H19" s="256"/>
-      <c r="I19" s="252">
-        <f>IF(H19="",D19*F19,D19*F19*H19)</f>
-        <v>1.2250000000000001</v>
+      <c r="H19" s="271">
+        <v>3</v>
+      </c>
+      <c r="I19" s="272">
+        <f t="shared" si="0"/>
+        <v>21.102</v>
       </c>
       <c r="J19" s="45"/>
       <c r="K19" s="45"/>
@@ -12218,19 +12614,29 @@
       <c r="O19" s="163"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="168"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="110" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="105">
-        <f>SUM(I16:I19)</f>
-        <v>57.534999999999997</v>
+      <c r="A20" s="273">
+        <v>50</v>
+      </c>
+      <c r="B20" s="247" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20" s="248" t="s">
+        <v>291</v>
+      </c>
+      <c r="D20" s="249">
+        <v>0.65</v>
+      </c>
+      <c r="E20" s="247" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="246">
+        <v>1</v>
+      </c>
+      <c r="G20" s="275"/>
+      <c r="H20" s="276"/>
+      <c r="I20" s="272">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
       </c>
       <c r="J20" s="45"/>
       <c r="K20" s="45"/>
@@ -12240,15 +12646,1622 @@
       <c r="O20" s="163"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="273">
+        <v>60</v>
+      </c>
+      <c r="B21" s="274" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="274" t="s">
+        <v>286</v>
+      </c>
+      <c r="D21" s="249">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="275" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="279">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G21" s="275"/>
+      <c r="H21" s="276"/>
+      <c r="I21" s="272">
+        <f t="shared" si="0"/>
+        <v>1.2350000000000001</v>
+      </c>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="163"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="168"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="280">
+        <f>SUM(I16:I21)</f>
+        <v>57.324999999999996</v>
+      </c>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="163"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="164"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="163"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="164"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="163"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="164"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="163"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="164"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="163"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="164"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="163"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="164"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="163"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="172"/>
+      <c r="B29" s="173"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="173"/>
+      <c r="E29" s="173"/>
+      <c r="F29" s="173"/>
+      <c r="G29" s="173"/>
+      <c r="H29" s="173"/>
+      <c r="I29" s="173"/>
+      <c r="J29" s="173"/>
+      <c r="K29" s="173"/>
+      <c r="L29" s="173"/>
+      <c r="M29" s="173"/>
+      <c r="N29" s="173"/>
+      <c r="O29" s="174"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I31" s="261"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H32" s="262"/>
+      <c r="J32" s="262"/>
+    </row>
+    <row r="33" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="262"/>
+    </row>
+    <row r="34" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F34" s="261"/>
+      <c r="G34" s="262"/>
+      <c r="H34" s="262"/>
+      <c r="J34" s="264"/>
+      <c r="K34" s="264"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" location="EN_A1000!A1" display="Driveshaft" xr:uid="{14C71347-ABED-4F3A-8B04-3EB2F1C5F84E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3129F321-BE68-4E0C-A8DD-7F6001EA6604}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="161"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="180" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="63">
+        <v>81</v>
+      </c>
+      <c r="L2" s="45"/>
+      <c r="M2" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="61">
+        <f>EN_1000_001_m+EN_1000_001_p</f>
+        <v>66.549787154500507</v>
+      </c>
+      <c r="O2" s="163"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="181" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="252" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="62">
+        <v>2</v>
+      </c>
+      <c r="O3" s="163"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="253" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="254" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="163"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="253" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="226" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="61">
+        <f>N3*N2</f>
+        <v>133.09957430900101</v>
+      </c>
+      <c r="O5" s="163"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="253" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="175" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="163"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="183" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="163"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="111"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="163"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="184"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="163"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="185" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="107" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="255" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="255" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="255" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="255" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="255" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="255" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="255" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="255" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="255" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="163"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="187">
+        <v>10</v>
+      </c>
+      <c r="B11" s="243" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" s="140">
+        <v>2.25</v>
+      </c>
+      <c r="E11" s="141">
+        <f>J11*K11*L11</f>
+        <v>4.2790580425663371</v>
+      </c>
+      <c r="F11" s="139" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="139"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="143" t="s">
+        <v>282</v>
+      </c>
+      <c r="J11" s="143">
+        <f>PI()*65.5*65.5/4/1000000</f>
+        <v>3.3695544705159026E-3</v>
+      </c>
+      <c r="K11" s="144">
+        <v>0.161773</v>
+      </c>
+      <c r="L11" s="145">
+        <v>7850</v>
+      </c>
+      <c r="M11" s="145">
+        <v>1</v>
+      </c>
+      <c r="N11" s="140">
+        <f>D11*J11*K11*L11*M11</f>
+        <v>9.6278805957742595</v>
+      </c>
+      <c r="O11" s="167"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="168"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="257" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="105">
+        <f>SUM(N11:N11)</f>
+        <v>9.6278805957742595</v>
+      </c>
+      <c r="O12" s="163"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="164"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="163"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="253" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="255" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="255" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="255" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="255" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="255" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="255" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="255" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="255" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="163"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="258">
+        <v>10</v>
+      </c>
+      <c r="B15" s="247" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="248" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="249">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="247" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="246">
+        <v>1</v>
+      </c>
+      <c r="G15" s="246"/>
+      <c r="H15" s="246"/>
+      <c r="I15" s="250">
+        <f>IF(H15="",D15*F15,D15*F15*H15)</f>
+        <v>1.3</v>
+      </c>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="163"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="259">
+        <v>20</v>
+      </c>
+      <c r="B16" s="248" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="248" t="s">
+        <v>287</v>
+      </c>
+      <c r="D16" s="249">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="263" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="251">
+        <v>313.90100000000001</v>
+      </c>
+      <c r="G16" s="265" t="s">
+        <v>288</v>
+      </c>
+      <c r="H16" s="266">
+        <v>3</v>
+      </c>
+      <c r="I16" s="250">
+        <f t="shared" ref="I16:I22" si="0">IF(H16="",D16*F16,D16*F16*H16)</f>
+        <v>37.668120000000002</v>
+      </c>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="163"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="258">
+        <v>30</v>
+      </c>
+      <c r="B17" s="247" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="248" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="249">
+        <v>0.65</v>
+      </c>
+      <c r="E17" s="247" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="246">
+        <v>1</v>
+      </c>
+      <c r="G17" s="246"/>
+      <c r="H17" s="246"/>
+      <c r="I17" s="250">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="163"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="268">
+        <v>40</v>
+      </c>
+      <c r="B18" s="269" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="269" t="s">
+        <v>289</v>
+      </c>
+      <c r="D18" s="249">
+        <v>0.04</v>
+      </c>
+      <c r="E18" s="270" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="278">
+        <v>161.94</v>
+      </c>
+      <c r="G18" s="265" t="s">
+        <v>288</v>
+      </c>
+      <c r="H18" s="271">
+        <v>3</v>
+      </c>
+      <c r="I18" s="272">
+        <f t="shared" si="0"/>
+        <v>19.4328</v>
+      </c>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="163"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="273">
+        <v>50</v>
+      </c>
+      <c r="B19" s="247" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="248" t="s">
+        <v>291</v>
+      </c>
+      <c r="D19" s="249">
+        <v>0.65</v>
+      </c>
+      <c r="E19" s="247" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="246">
+        <v>1</v>
+      </c>
+      <c r="G19" s="275"/>
+      <c r="H19" s="276"/>
+      <c r="I19" s="272">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="163"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="273">
+        <v>60</v>
+      </c>
+      <c r="B20" s="274" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="274" t="s">
+        <v>286</v>
+      </c>
+      <c r="D20" s="249">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="275" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="279">
+        <v>5.8928000000000003</v>
+      </c>
+      <c r="G20" s="275"/>
+      <c r="H20" s="276"/>
+      <c r="I20" s="272">
+        <f t="shared" si="0"/>
+        <v>2.9464000000000001</v>
+      </c>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="163"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="281">
+        <v>70</v>
+      </c>
+      <c r="B21" s="274" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="274" t="s">
+        <v>297</v>
+      </c>
+      <c r="D21" s="282">
+        <v>0.65</v>
+      </c>
+      <c r="E21" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="284">
+        <v>1</v>
+      </c>
+      <c r="G21" s="285"/>
+      <c r="H21" s="285"/>
+      <c r="I21" s="277">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="163"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="273">
+        <v>80</v>
+      </c>
+      <c r="B22" s="274" t="s">
+        <v>298</v>
+      </c>
+      <c r="C22" s="274" t="s">
+        <v>299</v>
+      </c>
+      <c r="D22" s="282">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="283" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="284">
+        <v>1.8452999999999999</v>
+      </c>
+      <c r="G22" s="285"/>
+      <c r="H22" s="285"/>
+      <c r="I22" s="277">
+        <f t="shared" si="0"/>
+        <v>0.18453</v>
+      </c>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="177"/>
+      <c r="M22" s="218"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="163"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="281"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="280">
+        <f>SUM(I15:I20)</f>
+        <v>62.647319999999993</v>
+      </c>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="163"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="163"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="45"/>
+      <c r="C25" s="267"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="163"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="45"/>
+      <c r="C26" s="177"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="163"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="287"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="163"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="163"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="163"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="173"/>
+      <c r="C30" s="173"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="173"/>
+      <c r="F30" s="173"/>
+      <c r="G30" s="173"/>
+      <c r="H30" s="173"/>
+      <c r="I30" s="173"/>
+      <c r="J30" s="173"/>
+      <c r="K30" s="173"/>
+      <c r="L30" s="173"/>
+      <c r="M30" s="173"/>
+      <c r="N30" s="173"/>
+      <c r="O30" s="174"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" location="EN_A1000!A1" display="Driveshaft" xr:uid="{FF9C9BF0-8081-401C-8903-0E5F32CF10C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58ABE86C-E34C-48C6-8181-74AE21A7D0A0}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="161"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="180" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="63">
+        <v>81</v>
+      </c>
+      <c r="L2" s="45"/>
+      <c r="M2" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="61">
+        <f>EN_1000_001_m+EN_1000_001_p</f>
+        <v>66.549787154500507</v>
+      </c>
+      <c r="O2" s="163"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="181" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="254" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="62">
+        <v>2</v>
+      </c>
+      <c r="O3" s="163"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="290" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="254" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="163"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="290" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="252" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="61">
+        <f>N3*N2</f>
+        <v>133.09957430900101</v>
+      </c>
+      <c r="O5" s="163"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="290" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="175" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="163"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="183" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="163"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="111"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="163"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="184"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="163"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="185" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="107" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="291" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="291" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="291" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="291" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="291" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="291" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="291" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="291" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="291" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="163"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="187">
+        <v>10</v>
+      </c>
+      <c r="B11" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="140">
+        <v>2.25</v>
+      </c>
+      <c r="E11" s="141">
+        <f>J11*K11*L11</f>
+        <v>1.1472790446544314</v>
+      </c>
+      <c r="F11" s="139" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="139"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="143" t="s">
+        <v>300</v>
+      </c>
+      <c r="J11" s="143">
+        <f>PI()*22.1*22.1/4/1000000</f>
+        <v>3.8359631698494783E-4</v>
+      </c>
+      <c r="K11" s="144">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="L11" s="145">
+        <v>7850</v>
+      </c>
+      <c r="M11" s="145">
+        <v>1</v>
+      </c>
+      <c r="N11" s="140">
+        <f>D11*J11*K11*L11*M11</f>
+        <v>2.58137785047247</v>
+      </c>
+      <c r="O11" s="167"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="168"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="293" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="105">
+        <f>SUM(N11:N11)</f>
+        <v>2.58137785047247</v>
+      </c>
+      <c r="O12" s="163"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="164"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="163"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="290" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="291" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="291" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="291" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="291" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="291" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="291" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="291" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="291" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="163"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="294">
+        <v>10</v>
+      </c>
+      <c r="B15" s="274" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="274" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="282">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="284">
+        <v>1</v>
+      </c>
+      <c r="G15" s="285"/>
+      <c r="H15" s="285"/>
+      <c r="I15" s="277">
+        <f>IF(H15="",D15*F15,D15*F15*H15)</f>
+        <v>1.3</v>
+      </c>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="163"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="294">
+        <v>20</v>
+      </c>
+      <c r="B16" s="274" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="274" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="282">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="283" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="288">
+        <f>J11*0.009249*2*1000000</f>
+        <v>7.0957646715875651</v>
+      </c>
+      <c r="G16" s="289" t="s">
+        <v>284</v>
+      </c>
+      <c r="H16" s="281">
+        <v>3</v>
+      </c>
+      <c r="I16" s="277">
+        <f>IF(H16="",D16*F16,D16*F16*H16)</f>
+        <v>0.8514917605905078</v>
+      </c>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="163"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="294">
+        <v>30</v>
+      </c>
+      <c r="B17" s="274" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="274" t="s">
+        <v>303</v>
+      </c>
+      <c r="D17" s="282">
+        <v>0.65</v>
+      </c>
+      <c r="E17" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="284">
+        <v>1</v>
+      </c>
+      <c r="G17" s="285"/>
+      <c r="H17" s="285"/>
+      <c r="I17" s="277">
+        <f>IF(H17="",D17*F17,D17*F17*H17)</f>
+        <v>0.65</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="163"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="294">
+        <v>40</v>
+      </c>
+      <c r="B18" s="274" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="274" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="282">
+        <v>0.04</v>
+      </c>
+      <c r="E18" s="283" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="288">
+        <f>(K11-2*0.009249)*PI()*0.00635*0.00635*1000000</f>
+        <v>45.920618646950281</v>
+      </c>
+      <c r="G18" s="289" t="s">
+        <v>284</v>
+      </c>
+      <c r="H18" s="281">
+        <v>3</v>
+      </c>
+      <c r="I18" s="277">
+        <f>IF(H18="",D18*F18,D18*F18*H18)</f>
+        <v>5.5104742376340337</v>
+      </c>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="163"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="294">
+        <v>50</v>
+      </c>
+      <c r="B19" s="274" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="274" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="282">
+        <v>0.65</v>
+      </c>
+      <c r="E19" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="284">
+        <v>1</v>
+      </c>
+      <c r="G19" s="285"/>
+      <c r="H19" s="285"/>
+      <c r="I19" s="277">
+        <f>IF(H19="",D19*F19,D19*F19*H19)</f>
+        <v>0.65</v>
+      </c>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="163"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="294">
+        <v>60</v>
+      </c>
+      <c r="B20" s="274" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="274" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="282">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="283" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="284">
+        <f>49.146*2/10</f>
+        <v>9.8292000000000002</v>
+      </c>
+      <c r="G20" s="285"/>
+      <c r="H20" s="285"/>
+      <c r="I20" s="277">
+        <f>IF(H20="",D20*F20,D20*F20*H20)</f>
+        <v>4.9146000000000001</v>
+      </c>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="163"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="164"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="280">
+        <f>SUM(I15:I20)</f>
+        <v>13.876565998224542</v>
+      </c>
       <c r="J21" s="45"/>
       <c r="K21" s="45"/>
       <c r="L21" s="45"/>
@@ -12290,6 +14303,772 @@
       <c r="N23" s="45"/>
       <c r="O23" s="163"/>
     </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="172"/>
+      <c r="B24" s="173"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="173"/>
+      <c r="J24" s="173"/>
+      <c r="K24" s="173"/>
+      <c r="L24" s="173"/>
+      <c r="M24" s="173"/>
+      <c r="N24" s="173"/>
+      <c r="O24" s="174"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" location="EN_A1000!A1" display="Driveshaft" xr:uid="{264BDC21-2F70-442B-B94A-24FE91BAB0E8}"/>
+    <hyperlink ref="D3" location="'EN_1000_003 Drawing'!A1" display="FileLink1" xr:uid="{E2643090-5EC8-4828-BDC3-2A60C67FB06D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5F5FF-3B9E-4BE6-BCC4-B605A4A577E2}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="286" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_1000_003" display="EN_1000_003" xr:uid="{0059A778-37A3-42B6-B92C-98F89F6D26F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6D7E70-3A36-4051-ADBC-E2E08B0C7EA8}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="159"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="161"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="179" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="180" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="63">
+        <v>81</v>
+      </c>
+      <c r="L2" s="45"/>
+      <c r="M2" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="61">
+        <f>EN_1000_001_m+EN_1000_001_p</f>
+        <v>66.549787154500507</v>
+      </c>
+      <c r="O2" s="163"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="181" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="254" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="62">
+        <v>2</v>
+      </c>
+      <c r="O3" s="163"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="290" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="254" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="163"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="290" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="252" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="61">
+        <f>N3*N2</f>
+        <v>133.09957430900101</v>
+      </c>
+      <c r="O5" s="163"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="290" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="175" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="163"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="183" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="163"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="179" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="111"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="163"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="184"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="163"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="185" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="107" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="107" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="291" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="291" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="291" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="291" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="291" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="291" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="291" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="291" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="291" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="163"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="187">
+        <v>10</v>
+      </c>
+      <c r="B11" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="140">
+        <v>2.25</v>
+      </c>
+      <c r="E11" s="141">
+        <f>J11*K11*L11</f>
+        <v>1.3002495839416888</v>
+      </c>
+      <c r="F11" s="139" t="s">
+        <v>155</v>
+      </c>
+      <c r="G11" s="139"/>
+      <c r="H11" s="142"/>
+      <c r="I11" s="143" t="s">
+        <v>300</v>
+      </c>
+      <c r="J11" s="143">
+        <f>PI()*22.1*22.1/4/1000000</f>
+        <v>3.8359631698494783E-4</v>
+      </c>
+      <c r="K11" s="144">
+        <v>0.43180000000000002</v>
+      </c>
+      <c r="L11" s="145">
+        <v>7850</v>
+      </c>
+      <c r="M11" s="145">
+        <v>1</v>
+      </c>
+      <c r="N11" s="140">
+        <f>D11*J11*K11*L11*M11</f>
+        <v>2.9255615638687997</v>
+      </c>
+      <c r="O11" s="167"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="168"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="293" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="105">
+        <f>SUM(N11:N11)</f>
+        <v>2.9255615638687997</v>
+      </c>
+      <c r="O12" s="163"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="164"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="163"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="290" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="291" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="291" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="291" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="291" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="291" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="291" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="291" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="291" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="163"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="294">
+        <v>10</v>
+      </c>
+      <c r="B15" s="274" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="274" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="282">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="284">
+        <v>1</v>
+      </c>
+      <c r="G15" s="285"/>
+      <c r="H15" s="285"/>
+      <c r="I15" s="277">
+        <f>IF(H15="",D15*F15,D15*F15*H15)</f>
+        <v>1.3</v>
+      </c>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="163"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="294">
+        <v>20</v>
+      </c>
+      <c r="B16" s="274" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="274" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="282">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="283" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="288">
+        <f>J11*0.014843*2*1000000</f>
+        <v>11.387440266015162</v>
+      </c>
+      <c r="G16" s="289" t="s">
+        <v>284</v>
+      </c>
+      <c r="H16" s="281">
+        <v>3</v>
+      </c>
+      <c r="I16" s="277">
+        <f>IF(H16="",D16*F16,D16*F16*H16)</f>
+        <v>1.3664928319218195</v>
+      </c>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="163"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="294">
+        <v>30</v>
+      </c>
+      <c r="B17" s="274" t="s">
+        <v>285</v>
+      </c>
+      <c r="C17" s="274" t="s">
+        <v>303</v>
+      </c>
+      <c r="D17" s="282">
+        <v>0.65</v>
+      </c>
+      <c r="E17" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="284">
+        <v>1</v>
+      </c>
+      <c r="G17" s="285"/>
+      <c r="H17" s="285"/>
+      <c r="I17" s="277">
+        <f>IF(H17="",D17*F17,D17*F17*H17)</f>
+        <v>0.65</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="163"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="294">
+        <v>40</v>
+      </c>
+      <c r="B18" s="274" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="274" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="282">
+        <v>0.04</v>
+      </c>
+      <c r="E18" s="283" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="288">
+        <f>(K11-2*0.014843)*PI()*0.00635*0.00635*1000000</f>
+        <v>50.938542812452809</v>
+      </c>
+      <c r="G18" s="289" t="s">
+        <v>284</v>
+      </c>
+      <c r="H18" s="281">
+        <v>3</v>
+      </c>
+      <c r="I18" s="277">
+        <f>IF(H18="",D18*F18,D18*F18*H18)</f>
+        <v>6.1126251374943372</v>
+      </c>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="163"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="294">
+        <v>50</v>
+      </c>
+      <c r="B19" s="274" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="274" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="282">
+        <v>0.65</v>
+      </c>
+      <c r="E19" s="283" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="284">
+        <v>1</v>
+      </c>
+      <c r="G19" s="285"/>
+      <c r="H19" s="285"/>
+      <c r="I19" s="277">
+        <f>IF(H19="",D19*F19,D19*F19*H19)</f>
+        <v>0.65</v>
+      </c>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="163"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="294">
+        <v>60</v>
+      </c>
+      <c r="B20" s="274" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="274" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="282">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="283" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="284">
+        <f>43.578*2/10</f>
+        <v>8.7156000000000002</v>
+      </c>
+      <c r="G20" s="285"/>
+      <c r="H20" s="285"/>
+      <c r="I20" s="277">
+        <f>IF(H20="",D20*F20,D20*F20*H20)</f>
+        <v>4.3578000000000001</v>
+      </c>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="163"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="164"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="280">
+        <f>SUM(I15:I20)</f>
+        <v>14.436917969416157</v>
+      </c>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="163"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="164"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="163"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="164"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="163"/>
+    </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="164"/>
       <c r="B24" s="45"/>
@@ -12324,43 +15103,115 @@
       <c r="N25" s="45"/>
       <c r="O25" s="163"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="164"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="163"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="172"/>
-      <c r="B27" s="173"/>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="173"/>
-      <c r="H27" s="173"/>
-      <c r="I27" s="173"/>
-      <c r="J27" s="173"/>
-      <c r="K27" s="173"/>
-      <c r="L27" s="173"/>
-      <c r="M27" s="173"/>
-      <c r="N27" s="173"/>
-      <c r="O27" s="174"/>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="172"/>
+      <c r="B26" s="173"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="173"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="173"/>
+      <c r="G26" s="173"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="173"/>
+      <c r="J26" s="173"/>
+      <c r="K26" s="173"/>
+      <c r="L26" s="173"/>
+      <c r="M26" s="173"/>
+      <c r="N26" s="173"/>
+      <c r="O26" s="174"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="45"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="45"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="45"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="EN_A1000!A1" display="Driveshaft" xr:uid="{14C71347-ABED-4F3A-8B04-3EB2F1C5F84E}"/>
+    <hyperlink ref="B4" location="EN_A1000!A1" display="Driveshaft" xr:uid="{58957493-CEF2-4EEA-B403-B9FA8EE073B4}"/>
+    <hyperlink ref="D3" location="'EN_1000_004 Drawing'!A1" display="FileLink1" xr:uid="{D079C1BA-582D-4B7A-BF47-41C78B6C2493}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AFD418-FC24-44FA-8188-943C3F051D67}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="EN_1000_004" display="EN_1000_004" xr:uid="{C9FAD0C7-A44C-434E-9009-46372571A36E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14287,7 +17138,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
COST DRIVETRAIN : on y croit !
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
+++ b/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Documents\ECL\EPSA\Github\EN - Engine &amp; Powertrain\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8E82EF-3999-49B6-9B28-6D7366D5D7C7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB4D54C-BB62-4483-916D-A89827F5C9C8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="21" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="21" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -1194,8 +1194,8 @@
     <numFmt numFmtId="174" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
     <numFmt numFmtId="175" formatCode="0.0000E+00"/>
     <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -2664,11 +2664,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFill="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="179" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="24" fillId="0" borderId="54" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -12852,7 +12852,7 @@
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -13655,8 +13655,8 @@
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14066,7 +14066,7 @@
       <c r="G15" s="285"/>
       <c r="H15" s="285"/>
       <c r="I15" s="277">
-        <f>IF(H15="",D15*F15,D15*F15*H15)</f>
+        <f t="shared" ref="I15:I20" si="0">IF(H15="",D15*F15,D15*F15*H15)</f>
         <v>1.3</v>
       </c>
       <c r="J15" s="45"/>
@@ -14093,8 +14093,8 @@
         <v>162</v>
       </c>
       <c r="F16" s="288">
-        <f>J11*0.009249*2*1000000</f>
-        <v>7.0957646715875651</v>
+        <f>J11*0.009891*2*1000000</f>
+        <v>7.5883023425962381</v>
       </c>
       <c r="G16" s="289" t="s">
         <v>284</v>
@@ -14103,8 +14103,8 @@
         <v>3</v>
       </c>
       <c r="I16" s="277">
-        <f>IF(H16="",D16*F16,D16*F16*H16)</f>
-        <v>0.8514917605905078</v>
+        <f t="shared" si="0"/>
+        <v>0.91059628111154867</v>
       </c>
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
@@ -14135,7 +14135,7 @@
       <c r="G17" s="285"/>
       <c r="H17" s="285"/>
       <c r="I17" s="277">
-        <f>IF(H17="",D17*F17,D17*F17*H17)</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="J17" s="45"/>
@@ -14162,8 +14162,8 @@
         <v>162</v>
       </c>
       <c r="F18" s="288">
-        <f>(K11-2*0.009249)*PI()*0.00635*0.00635*1000000</f>
-        <v>45.920618646950281</v>
+        <f>(K11-2*0.009891)*PI()*0.00635*0.00635*1000000</f>
+        <v>45.75796554615998</v>
       </c>
       <c r="G18" s="289" t="s">
         <v>284</v>
@@ -14172,8 +14172,8 @@
         <v>3</v>
       </c>
       <c r="I18" s="277">
-        <f>IF(H18="",D18*F18,D18*F18*H18)</f>
-        <v>5.5104742376340337</v>
+        <f t="shared" si="0"/>
+        <v>5.4909558655391972</v>
       </c>
       <c r="J18" s="45"/>
       <c r="K18" s="45"/>
@@ -14204,7 +14204,7 @@
       <c r="G19" s="285"/>
       <c r="H19" s="285"/>
       <c r="I19" s="277">
-        <f>IF(H19="",D19*F19,D19*F19*H19)</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="J19" s="45"/>
@@ -14237,7 +14237,7 @@
       <c r="G20" s="285"/>
       <c r="H20" s="285"/>
       <c r="I20" s="277">
-        <f>IF(H20="",D20*F20,D20*F20*H20)</f>
+        <f t="shared" si="0"/>
         <v>4.9146000000000001</v>
       </c>
       <c r="J20" s="45"/>
@@ -14260,7 +14260,7 @@
       </c>
       <c r="I21" s="280">
         <f>SUM(I15:I20)</f>
-        <v>13.876565998224542</v>
+        <v>13.916152146650747</v>
       </c>
       <c r="J21" s="45"/>
       <c r="K21" s="45"/>
@@ -14832,7 +14832,7 @@
       <c r="G15" s="285"/>
       <c r="H15" s="285"/>
       <c r="I15" s="277">
-        <f>IF(H15="",D15*F15,D15*F15*H15)</f>
+        <f t="shared" ref="I15:I20" si="0">IF(H15="",D15*F15,D15*F15*H15)</f>
         <v>1.3</v>
       </c>
       <c r="J15" s="45"/>
@@ -14869,7 +14869,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="277">
-        <f>IF(H16="",D16*F16,D16*F16*H16)</f>
+        <f t="shared" si="0"/>
         <v>1.3664928319218195</v>
       </c>
       <c r="J16" s="45"/>
@@ -14901,7 +14901,7 @@
       <c r="G17" s="285"/>
       <c r="H17" s="285"/>
       <c r="I17" s="277">
-        <f>IF(H17="",D17*F17,D17*F17*H17)</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="J17" s="45"/>
@@ -14938,7 +14938,7 @@
         <v>3</v>
       </c>
       <c r="I18" s="277">
-        <f>IF(H18="",D18*F18,D18*F18*H18)</f>
+        <f t="shared" si="0"/>
         <v>6.1126251374943372</v>
       </c>
       <c r="J18" s="45"/>
@@ -14970,7 +14970,7 @@
       <c r="G19" s="285"/>
       <c r="H19" s="285"/>
       <c r="I19" s="277">
-        <f>IF(H19="",D19*F19,D19*F19*H19)</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="J19" s="45"/>
@@ -15003,7 +15003,7 @@
       <c r="G20" s="285"/>
       <c r="H20" s="285"/>
       <c r="I20" s="277">
-        <f>IF(H20="",D20*F20,D20*F20*H20)</f>
+        <f t="shared" si="0"/>
         <v>4.3578000000000001</v>
       </c>
       <c r="J20" s="45"/>

</xml_diff>

<commit_message>
COST DRIVETRAIN : Differential Assy + Driveshaft Assy terminés (reste Chain Set)
</commit_message>
<xml_diff>
--- a/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
+++ b/EN - Engine & Powertrain/Cost/cost_drivetrain.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrien\Documents\ECL\EPSA\Github\EN - Engine &amp; Powertrain\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9CB367-115B-4F5B-A94F-C0F85E81CECF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8971BD-4DF2-4D2A-B61E-11E9EBCF00B4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="20" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" firstSheet="21" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -3446,6 +3446,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>732190</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>65803</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4356D1C9-02FC-480B-AA3F-3D20FD8E1932}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="333375"/>
+          <a:ext cx="9876190" cy="6971428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -3480,6 +3529,55 @@
         <a:xfrm>
           <a:off x="11706225" y="2628900"/>
           <a:ext cx="3342701" cy="1990026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>84489</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>56278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D690046-51DF-4C9D-9928-1667E8FC9ECB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="104775" y="323850"/>
+          <a:ext cx="9885714" cy="6971428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14398,7 +14496,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14413,6 +14511,7 @@
     <hyperlink ref="A1" location="EN_1000_003" display="EN_1000_003" xr:uid="{0059A778-37A3-42B6-B92C-98F89F6D26F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14423,8 +14522,8 @@
   </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15202,7 +15301,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15216,6 +15317,7 @@
     <hyperlink ref="A1" location="EN_1000_004" display="EN_1000_004" xr:uid="{C9FAD0C7-A44C-434E-9009-46372571A36E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>